<commit_message>
This is the second step in this project
</commit_message>
<xml_diff>
--- a/Automation/src/main/resources/userlogindetails1.xlsx
+++ b/Automation/src/main/resources/userlogindetails1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAI SRINIVAS\eclipse-workspace\Automation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAI SRINIVAS\git\repository\Automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6B17654-90F2-4D0B-B9C9-6F728C6163A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEEBF32-67F1-414C-B53D-BB2A48D2AFB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userlogs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>password1</t>
   </si>
@@ -90,19 +90,97 @@
     <t>Mobile</t>
   </si>
   <si>
-    <t>"1234567890"</t>
-  </si>
-  <si>
-    <t>"23-08-2000"</t>
-  </si>
-  <si>
-    <t>"24-08-2000"</t>
-  </si>
-  <si>
-    <t>"25-08-2000"</t>
-  </si>
-  <si>
-    <t>"26-08-2000"</t>
+    <t>23-08-2000</t>
+  </si>
+  <si>
+    <t>24-08-2000</t>
+  </si>
+  <si>
+    <t>25-08-2000</t>
+  </si>
+  <si>
+    <t>26-08-2000</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>1234567892</t>
+  </si>
+  <si>
+    <t>1234567893</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>123457</t>
+  </si>
+  <si>
+    <t>123458</t>
+  </si>
+  <si>
+    <t>123459</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>uwvd</t>
+  </si>
+  <si>
+    <t>product-collection-image-404</t>
+  </si>
+  <si>
+    <t>product-collection-image-417</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Royal Blue</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -153,14 +231,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,11 +536,15 @@
     <col min="3" max="3" width="30.88671875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="3"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -475,14 +560,41 @@
       <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -499,13 +611,40 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
         <v>21</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -522,13 +661,40 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -545,13 +711,40 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -568,10 +761,37 @@
         <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>